<commit_message>
First pass of 15 states
Did quick pass of 15 states. Updated xls with info and added csv where possible. In most cases need Spider. Was able to get estimate for kansas only.
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32037F24-A08B-4457-8A5E-0BD01DCDBFD4}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89AD868A-C3AA-4F0A-80C2-514E3C461212}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$G$51</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="138">
   <si>
     <t>Alabama</t>
   </si>
@@ -364,26 +367,95 @@
     <t>Son search</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>23 companies with daughter or daughters on it</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results capped at 2,000 and hard to copy/paste since only shows 20 per page. </t>
-  </si>
-  <si>
-    <t>Perhaps with a Spider/Crawler?</t>
+    <t>Needs spider</t>
+  </si>
+  <si>
+    <t>23 companies with daughter or daughters on it. Still need to do a regex</t>
+  </si>
+  <si>
+    <t>163 companies in 9 pages - need spider</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91 records found, copied into csv. </t>
+  </si>
+  <si>
+    <t>14240 records found in pages of 250 - need spider</t>
+  </si>
+  <si>
+    <t>Need spider - Found 309 matching record(s).  Viewing page 1 of 16.</t>
+  </si>
+  <si>
+    <t>Search not working since too many counts, need to hack it to limit son - Exceeded Record Count, please refine search</t>
+  </si>
+  <si>
+    <t>Results capped at 2,000 and hard to copy/paste since only shows 20 per page. Need spider.</t>
+  </si>
+  <si>
+    <t>Your Search Criteria returns 43783 results which is more than 500 results. Need to figure out how to get 500 son and then spider</t>
+  </si>
+  <si>
+    <t>Found 27 with DAUGHTER* &amp; 19 with *DAUGHTER. Already in one csv to get regex.</t>
+  </si>
+  <si>
+    <t>Found 677 with son* and 2955 with *son. Need spider and then dedup.</t>
+  </si>
+  <si>
+    <t>Found 33 and are in csv ready for regex</t>
+  </si>
+  <si>
+    <t>Only gives 50 when searching for son</t>
+  </si>
+  <si>
+    <t>return results but not counts, need spider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need spider - Page 2 of 21, records 26 to 50 of 513 </t>
+  </si>
+  <si>
+    <t>Need spider - Page 1 of 2558, records 1 to 25 of 63936</t>
+  </si>
+  <si>
+    <t>48 records on csv ready to regex</t>
+  </si>
+  <si>
+    <t>Has more button below table and each time it is clicked adds 10 records. Can we spider that?</t>
+  </si>
+  <si>
+    <t>Could copy/paste but spider would be better - Page 1 of 8, records 1 to 25 of 199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need spider - Page 1 of 1440, records 1 to 25 of 35979  </t>
+  </si>
+  <si>
+    <t>Could copy/paste but spider would be better - Results 1 - 25 of 74</t>
+  </si>
+  <si>
+    <t>son capped at 1000 results, sons capped at 1000 resuts. Need Spider - Results 1 - 25 of 1000</t>
+  </si>
+  <si>
+    <t>15 records found, easily copied to csv</t>
+  </si>
+  <si>
+    <t>results capped at 400 so searched for son and sons and rbind - 450-ish (need to dedup before regex)</t>
+  </si>
+  <si>
+    <t>Conservative Estimate</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>75/14 ~ 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +467,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -421,12 +501,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -996,182 +1081,244 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.7109375" customWidth="1"/>
-    <col min="6" max="6" width="71.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="71.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G1" t="s">
-        <v>110</v>
+      <c r="G1" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>67</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1179,231 +1326,270 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1411,10 +1597,10 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1422,10 +1608,10 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1433,10 +1619,10 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1444,13 +1630,13 @@
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1458,10 +1644,10 @@
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1469,13 +1655,13 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1483,13 +1669,13 @@
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1497,10 +1683,10 @@
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1508,10 +1694,10 @@
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1519,10 +1705,10 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1530,10 +1716,10 @@
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1541,10 +1727,10 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1552,10 +1738,10 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1563,10 +1749,10 @@
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1574,10 +1760,10 @@
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1585,13 +1771,13 @@
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1599,10 +1785,10 @@
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1610,13 +1796,13 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1624,16 +1810,27 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{57FE75D0-032C-4AC1-83C8-CCA0DEF7DD1E}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{DAAD63D8-7315-40FF-A6E5-CCD3001C4F5B}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{5239234C-285F-44D2-A707-D31FE2E9A5C9}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{0B2344C5-ADDD-4D77-B4A3-CD4458D0B8CC}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{4914C519-EAE7-4913-9B1C-C7BBF8E6B38B}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{232C81D9-1E87-4C16-B61C-56CB858473FB}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{8058C86F-AD88-40CA-A816-C894C82DDCCD}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{501D0F09-5707-41B2-9F84-0072E94D0FCE}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{9D44CC03-093F-4F7E-8E5B-F0624B178431}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{15B65C99-090A-4014-8BC9-47AA25ABB5BD}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{59ABBE2F-E96D-447A-A8BE-658D5BBCEBB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
KY - MA pass 1 done
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C78659B1-433A-4275-94E5-9C1DD6899630}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFB22B89-634A-4500-AA19-833AFA088E01}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
   <si>
     <t>Alabama</t>
   </si>
@@ -452,16 +452,41 @@
   </si>
   <si>
     <t>only allows 250 results and requires 4 characters. Sons return 75, "son " returns 249 so I rbind (324) them and them dedup before estimate</t>
+  </si>
+  <si>
+    <t>250 in 10 pages, need spider</t>
+  </si>
+  <si>
+    <t>Capped at 250 in 10 pages, need spider</t>
+  </si>
+  <si>
+    <t>53 found and copied to csv</t>
+  </si>
+  <si>
+    <t>Results capped at 100. So got 100 sons and 100 son then rbind and then dedup</t>
+  </si>
+  <si>
+    <t>84 rows found, easily copied to csv</t>
+  </si>
+  <si>
+    <t>capped at 400, so rbind 400 son and 172 sons, then dedup</t>
+  </si>
+  <si>
+    <t>Using "full text" search found 29 daugther and 119 daughters records. Removed empty lines and dedup</t>
+  </si>
+  <si>
+    <t>Using "full text" search found 2154 son and 3902 sons records. Removed emplty lines and dedup.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +504,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -503,11 +535,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -518,11 +551,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1090,8 +1130,8 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,8 +1142,9 @@
     <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="71.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="18.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1125,7 +1166,7 @@
       <c r="F1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1424,7 +1465,7 @@
       <c r="F17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="5">
         <f>75/14</f>
         <v>5.3571428571428568</v>
       </c>
@@ -1448,7 +1489,7 @@
       <c r="F18" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="5">
         <f>66/16</f>
         <v>4.125</v>
       </c>
@@ -1460,8 +1501,17 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>89</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,8 +1521,21 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>91</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="6">
+        <f>45/52</f>
+        <v>0.86538461538461542</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,19 +1545,45 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G21" s="5">
+        <f>128/82</f>
+        <v>1.5609756097560976</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>95</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="5">
+        <f>5979/147</f>
+        <v>40.673469387755105</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1856,6 +1945,10 @@
     <hyperlink ref="C17" r:id="rId11" xr:uid="{59ABBE2F-E96D-447A-A8BE-658D5BBCEBB9}"/>
     <hyperlink ref="C11" r:id="rId12" xr:uid="{52AB6CA7-2C51-483E-AB81-D8C456E36E4E}"/>
     <hyperlink ref="C18" r:id="rId13" xr:uid="{8CE5F8D3-2664-47BC-AC92-CC2AFB1F86E1}"/>
+    <hyperlink ref="C19" r:id="rId14" xr:uid="{883FB522-98B0-4142-BAA1-CA9467FA04BB}"/>
+    <hyperlink ref="C20" r:id="rId15" xr:uid="{668DB339-8157-4A7C-98BE-A963E1B2D647}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{2EE67D5C-E95F-4BFA-8D94-1228F2F52D7D}"/>
+    <hyperlink ref="C22" r:id="rId17" xr:uid="{F8B3B7AF-6AE0-4640-B0B9-FFBE5B89099C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First pass until OK completed.
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7355ddd88330403a/Documents/GitHub/sonny_side/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFB22B89-634A-4500-AA19-833AFA088E01}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A801DAAC-B54C-49CE-81B8-C83F6143B379}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="171">
   <si>
     <t>Alabama</t>
   </si>
@@ -476,6 +476,78 @@
   </si>
   <si>
     <t>Using "full text" search found 2154 son and 3902 sons records. Removed emplty lines and dedup.</t>
+  </si>
+  <si>
+    <t>Annoying copy/paste generated 3 rows per company so prepared in xls. Had to search for daughter for active and inactive separately. 219 in CSV.</t>
+  </si>
+  <si>
+    <t>Capped at 500. Searched 4 times and rbind results for son &amp; sons vs. active/inactive. 2000 in CSV. Dedup in R.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Very conservative since only got son coverage until letter d. Could redo and include starts with son but spider might be better</t>
+  </si>
+  <si>
+    <t>Search gives counts with exact match.</t>
+  </si>
+  <si>
+    <t>Spider needed if we want data in R</t>
+  </si>
+  <si>
+    <t>Need spider</t>
+  </si>
+  <si>
+    <t>41 rows found and copy/pasted to csv</t>
+  </si>
+  <si>
+    <t>?/41</t>
+  </si>
+  <si>
+    <t>keyword search of son gives error. Sons keyword search returns 1390 but really need spider</t>
+  </si>
+  <si>
+    <t>120 contain daughter but need spider</t>
+  </si>
+  <si>
+    <t>15506 contain son but need spider</t>
+  </si>
+  <si>
+    <t>74 contain daughter, need spider</t>
+  </si>
+  <si>
+    <t>Caps at 500, need spider</t>
+  </si>
+  <si>
+    <t>52 contain daughter, need spider</t>
+  </si>
+  <si>
+    <t>7861 contain son, need spider</t>
+  </si>
+  <si>
+    <t>261 contain daughter, need spider</t>
+  </si>
+  <si>
+    <t>1930 contain son, need spider</t>
+  </si>
+  <si>
+    <t>230 contain daughter, need spider</t>
+  </si>
+  <si>
+    <t>asks for min of 4 characters son can't search for son. Sons capped at 500</t>
+  </si>
+  <si>
+    <t>22 contain daughter but how to parse</t>
+  </si>
+  <si>
+    <t>Caps at 500 so need multiple searches. How to parse these results so I don't copy/paste oddly from xls</t>
+  </si>
+  <si>
+    <t>174 contain daughter, need spider</t>
+  </si>
+  <si>
+    <t>son capped at 500, sons cap at 500. need spider</t>
   </si>
 </sst>
 </file>
@@ -484,7 +556,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -551,13 +623,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1127,11 +1199,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE50C96B-AE9B-4FF9-A241-178704DDBFF3}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,11 +1215,11 @@
     <col min="5" max="5" width="51.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="71.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>105</v>
       </c>
@@ -1169,8 +1241,11 @@
       <c r="G1" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1184,7 +1259,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1204,7 +1279,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1224,7 +1299,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1244,7 +1319,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1258,7 +1333,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1278,7 +1353,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1298,7 +1373,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1318,7 +1393,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1338,7 +1413,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1358,7 +1433,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1372,7 +1447,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1386,7 +1461,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1406,7 +1481,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1426,7 +1501,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1446,7 +1521,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1470,7 +1545,7 @@
         <v>5.3571428571428568</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1494,7 +1569,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1514,7 +1589,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1538,7 +1613,7 @@
         <v>0.86538461538461542</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1562,7 +1637,7 @@
         <v>1.5609756097560976</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1586,7 +1661,7 @@
         <v>40.673469387755105</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1600,40 +1675,81 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="5">
+        <f>222/212</f>
+        <v>1.0471698113207548</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" s="5">
+        <f>752/22</f>
+        <v>34.18181818181818</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1647,18 +1763,30 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1672,62 +1800,107 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1737,8 +1910,17 @@
       <c r="C35" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1752,18 +1934,27 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1777,7 +1968,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1791,7 +1982,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1802,7 +1993,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1813,7 +2004,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1824,7 +2015,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1835,7 +2026,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1846,7 +2037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1857,7 +2048,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1868,7 +2059,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1879,7 +2070,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1949,6 +2140,16 @@
     <hyperlink ref="C20" r:id="rId15" xr:uid="{668DB339-8157-4A7C-98BE-A963E1B2D647}"/>
     <hyperlink ref="C21" r:id="rId16" xr:uid="{2EE67D5C-E95F-4BFA-8D94-1228F2F52D7D}"/>
     <hyperlink ref="C22" r:id="rId17" xr:uid="{F8B3B7AF-6AE0-4640-B0B9-FFBE5B89099C}"/>
+    <hyperlink ref="C24" r:id="rId18" xr:uid="{41B67C76-9DC2-4056-ADBA-E03069095849}"/>
+    <hyperlink ref="C25" r:id="rId19" location="clear=1" xr:uid="{2BEEAB08-8AFB-4EE1-9899-E43718836604}"/>
+    <hyperlink ref="C26" r:id="rId20" xr:uid="{BB238253-F355-4A5C-9AB8-1FA662EAD62F}"/>
+    <hyperlink ref="C28" r:id="rId21" xr:uid="{E5666281-7B26-4687-BB28-2199900A1080}"/>
+    <hyperlink ref="C30" r:id="rId22" xr:uid="{4C2BA448-D508-48B1-8ECE-E95B7EE8E697}"/>
+    <hyperlink ref="C31" r:id="rId23" xr:uid="{24C173A1-C8FC-446E-9A50-C963EA681A61}"/>
+    <hyperlink ref="C32" r:id="rId24" xr:uid="{FFDBBC53-FE5C-4074-8C48-F2A462425E55}"/>
+    <hyperlink ref="C34" r:id="rId25" xr:uid="{17C89D37-87D2-4E18-94CD-87AB8270DAEE}"/>
+    <hyperlink ref="C33" r:id="rId26" xr:uid="{66CAB1C1-B412-428E-A26F-76605F6594E4}"/>
+    <hyperlink ref="C37" r:id="rId27" xr:uid="{4F43174A-9092-4809-8B80-B1CE410EBA31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First pass of 50 states done
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7355ddd88330403a/Documents/GitHub/sonny_side/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A801DAAC-B54C-49CE-81B8-C83F6143B379}"/>
+  <xr:revisionPtr revIDLastSave="323" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F4FCD5B-F8A8-4D1E-9930-022B67BC3F87}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$G$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="188">
   <si>
     <t>Alabama</t>
   </si>
@@ -73,9 +72,6 @@
     <t>Idaho</t>
   </si>
   <si>
-    <t>IllinoisIndiana</t>
-  </si>
-  <si>
     <t>Iowa</t>
   </si>
   <si>
@@ -109,9 +105,6 @@
     <t>Missouri</t>
   </si>
   <si>
-    <t>MontanaNebraska</t>
-  </si>
-  <si>
     <t>Nevada</t>
   </si>
   <si>
@@ -142,9 +135,6 @@
     <t>Oregon</t>
   </si>
   <si>
-    <t>PennsylvaniaRhode Island</t>
-  </si>
-  <si>
     <t>South Carolina</t>
   </si>
   <si>
@@ -548,6 +538,66 @@
   </si>
   <si>
     <t>son capped at 500, sons cap at 500. need spider</t>
+  </si>
+  <si>
+    <t>Had to do 3 different searches: begins with, full text, inactive. 12 rows in csv to R</t>
+  </si>
+  <si>
+    <t>Had to do 3 different searches: begins with, full text, inactive. 314 rows in csv to R</t>
+  </si>
+  <si>
+    <t>173 contain daughter but only 60 are shown. Copy paste ok</t>
+  </si>
+  <si>
+    <t>27222 have "son" but only 60 are shown. Copy paste ok</t>
+  </si>
+  <si>
+    <t>9/60 for son were true positive so extrapolate</t>
+  </si>
+  <si>
+    <t>had to search twice (contains vs starts with) to get more results. Will dedup in R.</t>
+  </si>
+  <si>
+    <t>Was able to search "contains" and got 141. Copy pasted ok to csv</t>
+  </si>
+  <si>
+    <t>Caps at 500 and displays 100 per page so need spider. Could do multiple searches to increase n results</t>
+  </si>
+  <si>
+    <t>daughter search would yield 221 but doesn't show. Daughters show 152 results.</t>
+  </si>
+  <si>
+    <t>son would yield 4,740 but doesn't show. Sons would yiled 275 but doesn't show</t>
+  </si>
+  <si>
+    <t>son yields 690 results in 14 pages. Need spider</t>
+  </si>
+  <si>
+    <t>daughter yields 17 results but copy/paste not working. Maybe spider?</t>
+  </si>
+  <si>
+    <t>65 rows copy pasted to csv</t>
+  </si>
+  <si>
+    <t>7393 results in 296 pages contain son, need spider</t>
+  </si>
+  <si>
+    <t>Page 1 of 12, records 1 to 25 of 278 -- need spider</t>
+  </si>
+  <si>
+    <t>Your Search Criteria returns 29121 results which is more than 500 results. Need to figure out how to hack to 500 and then extrapolate. Needs spider</t>
+  </si>
+  <si>
+    <t>76 results in 8 pages, spider would be best</t>
+  </si>
+  <si>
+    <t>shows up to 1000 results in pages of 10 - ouch. Needs spider</t>
+  </si>
+  <si>
+    <t>40 results found but copy/paste is not working</t>
+  </si>
+  <si>
+    <t>10294 results in 515 pages. Need spider</t>
   </si>
 </sst>
 </file>
@@ -947,263 +997,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6255719F-7F7C-42A0-85CA-239E3A176C0E}">
-  <dimension ref="A1:A47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE50C96B-AE9B-4FF9-A241-178704DDBFF3}">
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,28 +1020,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1253,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1267,16 +1066,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1287,16 +1086,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1307,16 +1106,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1327,10 +1126,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1341,16 +1140,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1361,16 +1160,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1381,16 +1180,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1401,16 +1200,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1421,16 +1220,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1441,10 +1240,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1455,10 +1254,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1466,19 +1265,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1486,19 +1285,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1506,19 +1305,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1526,19 +1325,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G17" s="5">
         <f>75/14</f>
@@ -1550,19 +1349,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G18" s="5">
         <f>66/16</f>
@@ -1574,19 +1373,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1594,19 +1393,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G20" s="6">
         <f>45/52</f>
@@ -1618,19 +1417,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G21" s="5">
         <f>128/82</f>
@@ -1642,19 +1441,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G22" s="5">
         <f>5979/147</f>
@@ -1666,13 +1465,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1680,26 +1479,26 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G24" s="5">
         <f>222/212</f>
         <v>1.0471698113207548</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1707,26 +1506,26 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G25" s="5">
         <f>752/22</f>
         <v>34.18181818181818</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1734,19 +1533,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1754,13 +1553,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1768,22 +1567,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1791,13 +1590,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1805,19 +1604,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1825,19 +1624,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1845,279 +1644,384 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G40" s="5">
+        <f>206/12</f>
+        <v>17.166666666666668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" s="5">
+        <f>(27222*9/60)/59</f>
+        <v>69.208474576271186</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G42" s="5">
+        <f>129/11</f>
+        <v>11.727272727272727</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>104</v>
+        <v>43</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2150,6 +2054,17 @@
     <hyperlink ref="C34" r:id="rId25" xr:uid="{17C89D37-87D2-4E18-94CD-87AB8270DAEE}"/>
     <hyperlink ref="C33" r:id="rId26" xr:uid="{66CAB1C1-B412-428E-A26F-76605F6594E4}"/>
     <hyperlink ref="C37" r:id="rId27" xr:uid="{4F43174A-9092-4809-8B80-B1CE410EBA31}"/>
+    <hyperlink ref="C35" r:id="rId28" xr:uid="{0973DD32-FE77-49EC-A8A9-AAA722E88CAE}"/>
+    <hyperlink ref="C40" r:id="rId29" xr:uid="{9C54D993-F061-41F1-8F41-5541B78A6CF3}"/>
+    <hyperlink ref="C41" r:id="rId30" xr:uid="{68EF8942-6A9F-43A0-9B77-6C5BC0EF57E6}"/>
+    <hyperlink ref="C42" r:id="rId31" xr:uid="{ADE95A00-F8D2-4BEC-B973-525C7559C5B8}"/>
+    <hyperlink ref="C43" r:id="rId32" xr:uid="{54DF2E61-CD6E-46DE-AE5E-085F446DDB64}"/>
+    <hyperlink ref="C44" r:id="rId33" xr:uid="{57729F6F-298E-414A-85D8-A01E33AC8146}"/>
+    <hyperlink ref="C45" r:id="rId34" xr:uid="{CCAEA818-7FE4-4B74-81A4-E2174150131D}"/>
+    <hyperlink ref="C46" r:id="rId35" xr:uid="{3DCF6AE2-80CD-4326-8C4A-074CDC77B77D}"/>
+    <hyperlink ref="C47" r:id="rId36" xr:uid="{B16EC75D-1255-473E-BF41-4BEAFF1CB6C6}"/>
+    <hyperlink ref="C49" r:id="rId37" xr:uid="{216EABAD-1D44-4AC9-832A-4D8D02FC6022}"/>
+    <hyperlink ref="C51" r:id="rId38" location="&amp;&amp;D1XZLnCoo8Z0jHfshWy070zSzxdxFoNyojR7wLtsqBKXma2Biw1bPoNQ35FIlZ20OZFVPPWKm2NVjBEWid89Yl+5G1w9meYdtfsLaZvHbBvHz8jdUMP8SPwa2hhoYyoDM9h6+eiuYPSH9xhY49fqg35E6OgRxfcg1iJxtfHylJBLsGD1" xr:uid="{FC6108CD-C840-4B86-AA75-9AE510F8ABE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CT done and FL work in progress
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7355ddd88330403a/Documents/GitHub/sonny_side/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="323" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F4FCD5B-F8A8-4D1E-9930-022B67BC3F87}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FBC794DB-31EB-4878-97B8-90F392B5A3BD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="189">
   <si>
     <t>Alabama</t>
   </si>
@@ -387,12 +387,6 @@
     <t>Your Search Criteria returns 43783 results which is more than 500 results. Need to figure out how to get 500 son and then spider</t>
   </si>
   <si>
-    <t>Found 27 with DAUGHTER* &amp; 19 with *DAUGHTER. Already in one csv to get regex.</t>
-  </si>
-  <si>
-    <t>Found 677 with son* and 2955 with *son. Need spider and then dedup.</t>
-  </si>
-  <si>
     <t>Found 33 and are in csv ready for regex</t>
   </si>
   <si>
@@ -598,6 +592,15 @@
   </si>
   <si>
     <t>10294 results in 515 pages. Need spider</t>
+  </si>
+  <si>
+    <t>Can't get any contents</t>
+  </si>
+  <si>
+    <t>Found 27 with DAUGHTER* &amp; 19 with *DAUGHTER. Copied easily to CSV</t>
+  </si>
+  <si>
+    <t>Found 679 with son* and 2954 with *son. Was able to relatively easy copy/paste in xls and then dedup in R</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1004,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,10 +1041,10 @@
         <v>106</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1069,13 +1072,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1163,13 +1169,17 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>117</v>
+        <v>187</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>118</v>
+        <v>188</v>
+      </c>
+      <c r="G8" s="5">
+        <f>875/43</f>
+        <v>20.348837209302324</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1186,10 +1196,10 @@
         <v>110</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1206,10 +1216,10 @@
         <v>107</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1226,10 +1236,10 @@
         <v>107</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1274,10 +1284,10 @@
         <v>110</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1294,10 +1304,10 @@
         <v>107</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1314,10 +1324,10 @@
         <v>107</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1331,13 +1341,13 @@
         <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G17" s="5">
         <f>75/14</f>
@@ -1355,13 +1365,13 @@
         <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G18" s="5">
         <f>66/16</f>
@@ -1382,10 +1392,10 @@
         <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1399,13 +1409,13 @@
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G20" s="6">
         <f>45/52</f>
@@ -1423,13 +1433,13 @@
         <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G21" s="5">
         <f>128/82</f>
@@ -1447,13 +1457,13 @@
         <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G22" s="5">
         <f>5979/147</f>
@@ -1488,17 +1498,17 @@
         <v>107</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G24" s="5">
         <f>222/212</f>
         <v>1.0471698113207548</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1515,17 +1525,17 @@
         <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G25" s="5">
         <f>752/22</f>
         <v>34.18181818181818</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1542,10 +1552,10 @@
         <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1576,13 +1586,13 @@
         <v>107</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="G28" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1613,10 +1623,10 @@
         <v>107</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1633,10 +1643,10 @@
         <v>107</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1653,10 +1663,10 @@
         <v>107</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,10 +1683,10 @@
         <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1693,10 +1703,10 @@
         <v>107</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1713,10 +1723,10 @@
         <v>110</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,10 +1757,10 @@
         <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,13 +1802,13 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G40" s="5">
         <f>206/12</f>
@@ -1816,20 +1826,20 @@
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G41" s="5">
         <f>(27222*9/60)/59</f>
         <v>69.208474576271186</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1843,13 +1853,13 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G42" s="5">
         <f>129/11</f>
@@ -1870,10 +1880,10 @@
         <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1890,10 +1900,10 @@
         <v>110</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1910,10 +1920,10 @@
         <v>107</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1930,10 +1940,10 @@
         <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1950,10 +1960,10 @@
         <v>107</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1984,10 +1994,10 @@
         <v>107</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,10 +2028,10 @@
         <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
de and fl -- done
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7355ddd88330403a/Documents/GitHub/sonny_side/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FBC794DB-31EB-4878-97B8-90F392B5A3BD}"/>
+  <xr:revisionPtr revIDLastSave="372" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7297B84C-D7E6-43A6-8F09-73F6DF27575A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="195">
   <si>
     <t>Alabama</t>
   </si>
@@ -378,9 +378,6 @@
     <t>Need spider - Found 309 matching record(s).  Viewing page 1 of 16.</t>
   </si>
   <si>
-    <t>Search not working since too many counts, need to hack it to limit son - Exceeded Record Count, please refine search</t>
-  </si>
-  <si>
     <t>Results capped at 2,000 and hard to copy/paste since only shows 20 per page. Need spider.</t>
   </si>
   <si>
@@ -390,12 +387,6 @@
     <t>Found 33 and are in csv ready for regex</t>
   </si>
   <si>
-    <t>Only gives 50 when searching for son</t>
-  </si>
-  <si>
-    <t>return results but not counts, need spider</t>
-  </si>
-  <si>
     <t xml:space="preserve">Need spider - Page 2 of 21, records 26 to 50 of 513 </t>
   </si>
   <si>
@@ -594,13 +585,40 @@
     <t>10294 results in 515 pages. Need spider</t>
   </si>
   <si>
-    <t>Can't get any contents</t>
-  </si>
-  <si>
     <t>Found 27 with DAUGHTER* &amp; 19 with *DAUGHTER. Copied easily to CSV</t>
   </si>
   <si>
     <t>Found 679 with son* and 2954 with *son. Was able to relatively easy copy/paste in xls and then dedup in R</t>
+  </si>
+  <si>
+    <t>Can't get rvest to run even with Gaurav generated URL</t>
+  </si>
+  <si>
+    <t>Need to figure out how to create customized URL to use rvest - help!</t>
+  </si>
+  <si>
+    <t>Could copy/paste since pages are 250 long but better if I can create customized url to rvest</t>
+  </si>
+  <si>
+    <t>Only works with searches of 500 or less results so need to trim/hack. Results in 30 pages so need spider</t>
+  </si>
+  <si>
+    <t>I do get URL to crawl but get nothing in R. not sure why? See R for code and links.</t>
+  </si>
+  <si>
+    <t>Only gives 50 results per search so I got 100 (son &amp; sons) search. I can't hack more results</t>
+  </si>
+  <si>
+    <t>CAUTION: Use carefuly since son is super under represented. I Just can't get more than 50 searches of son</t>
+  </si>
+  <si>
+    <t>9 links parsed with spider</t>
+  </si>
+  <si>
+    <t>100+ links parsed with spider</t>
+  </si>
+  <si>
+    <t>horrible excercse since links have to be hard coded. Use with CAUTION since only searches that start with daughter and son were allowed. Couldn't search for *daughter or *son unfortunately. Results are very partial.</t>
   </si>
 </sst>
 </file>
@@ -665,7 +683,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -685,6 +703,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1001,11 +1020,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE50C96B-AE9B-4FF9-A241-178704DDBFF3}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,13 +1061,13 @@
         <v>106</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1061,7 +1081,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1078,13 +1098,13 @@
         <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1101,10 +1121,13 @@
         <v>109</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1115,7 +1138,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>111</v>
@@ -1123,8 +1146,11 @@
       <c r="F5" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1138,7 +1164,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1155,10 +1181,13 @@
         <v>113</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1169,20 +1198,20 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G8" s="5">
         <f>875/43</f>
         <v>20.348837209302324</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1193,33 +1222,47 @@
         <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="G9" s="5">
+        <f>24/33</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>119</v>
+        <v>192</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>119</v>
+        <v>193</v>
+      </c>
+      <c r="G10" s="5">
+        <f>729/176</f>
+        <v>4.1420454545454541</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1236,13 +1279,13 @@
         <v>107</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1256,7 +1299,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1270,7 +1313,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1284,13 +1327,13 @@
         <v>110</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1304,13 +1347,13 @@
         <v>107</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1324,13 +1367,13 @@
         <v>107</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1341,20 +1384,20 @@
         <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G17" s="5">
         <f>75/14</f>
         <v>5.3571428571428568</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1365,20 +1408,20 @@
         <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G18" s="5">
         <f>66/16</f>
         <v>4.125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1392,13 +1435,13 @@
         <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1409,20 +1452,20 @@
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G20" s="6">
         <f>45/52</f>
         <v>0.86538461538461542</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1433,20 +1476,20 @@
         <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G21" s="5">
         <f>128/82</f>
         <v>1.5609756097560976</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1457,20 +1500,20 @@
         <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G22" s="5">
         <f>5979/147</f>
         <v>40.673469387755105</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1484,7 +1527,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1498,20 +1541,20 @@
         <v>107</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G24" s="5">
         <f>222/212</f>
         <v>1.0471698113207548</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1525,20 +1568,20 @@
         <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G25" s="5">
         <f>752/22</f>
         <v>34.18181818181818</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1552,13 +1595,13 @@
         <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1572,7 +1615,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1586,16 +1629,16 @@
         <v>107</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1609,7 +1652,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1623,13 +1666,13 @@
         <v>107</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1643,13 +1686,13 @@
         <v>107</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1663,13 +1706,13 @@
         <v>107</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1683,13 +1726,13 @@
         <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1703,13 +1746,13 @@
         <v>107</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1723,13 +1766,13 @@
         <v>110</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1743,7 +1786,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1757,13 +1800,13 @@
         <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1777,7 +1820,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1791,7 +1834,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1802,20 +1845,20 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G40" s="5">
         <f>206/12</f>
         <v>17.166666666666668</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1826,23 +1869,23 @@
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G41" s="5">
         <f>(27222*9/60)/59</f>
         <v>69.208474576271186</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1853,20 +1896,20 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G42" s="5">
         <f>129/11</f>
         <v>11.727272727272727</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1880,13 +1923,13 @@
         <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1900,13 +1943,13 @@
         <v>110</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1920,13 +1963,13 @@
         <v>107</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1940,13 +1983,13 @@
         <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1960,13 +2003,13 @@
         <v>107</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1980,7 +2023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1994,13 +2037,13 @@
         <v>107</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2014,7 +2057,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2028,14 +2071,26 @@
         <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}"/>
+  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="10"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Blocked"/>
+        <filter val="Needs spider"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{57FE75D0-032C-4AC1-83C8-CCA0DEF7DD1E}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{DAAD63D8-7315-40FF-A6E5-CCD3001C4F5B}"/>
@@ -2043,38 +2098,38 @@
     <hyperlink ref="C7" r:id="rId4" xr:uid="{0B2344C5-ADDD-4D77-B4A3-CD4458D0B8CC}"/>
     <hyperlink ref="C8" r:id="rId5" xr:uid="{4914C519-EAE7-4913-9B1C-C7BBF8E6B38B}"/>
     <hyperlink ref="C9" r:id="rId6" xr:uid="{232C81D9-1E87-4C16-B61C-56CB858473FB}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{8058C86F-AD88-40CA-A816-C894C82DDCCD}"/>
-    <hyperlink ref="C14" r:id="rId8" xr:uid="{501D0F09-5707-41B2-9F84-0072E94D0FCE}"/>
-    <hyperlink ref="C15" r:id="rId9" xr:uid="{9D44CC03-093F-4F7E-8E5B-F0624B178431}"/>
-    <hyperlink ref="C16" r:id="rId10" xr:uid="{15B65C99-090A-4014-8BC9-47AA25ABB5BD}"/>
-    <hyperlink ref="C17" r:id="rId11" xr:uid="{59ABBE2F-E96D-447A-A8BE-658D5BBCEBB9}"/>
-    <hyperlink ref="C11" r:id="rId12" xr:uid="{52AB6CA7-2C51-483E-AB81-D8C456E36E4E}"/>
-    <hyperlink ref="C18" r:id="rId13" xr:uid="{8CE5F8D3-2664-47BC-AC92-CC2AFB1F86E1}"/>
-    <hyperlink ref="C19" r:id="rId14" xr:uid="{883FB522-98B0-4142-BAA1-CA9467FA04BB}"/>
-    <hyperlink ref="C20" r:id="rId15" xr:uid="{668DB339-8157-4A7C-98BE-A963E1B2D647}"/>
-    <hyperlink ref="C21" r:id="rId16" xr:uid="{2EE67D5C-E95F-4BFA-8D94-1228F2F52D7D}"/>
-    <hyperlink ref="C22" r:id="rId17" xr:uid="{F8B3B7AF-6AE0-4640-B0B9-FFBE5B89099C}"/>
-    <hyperlink ref="C24" r:id="rId18" xr:uid="{41B67C76-9DC2-4056-ADBA-E03069095849}"/>
-    <hyperlink ref="C25" r:id="rId19" location="clear=1" xr:uid="{2BEEAB08-8AFB-4EE1-9899-E43718836604}"/>
-    <hyperlink ref="C26" r:id="rId20" xr:uid="{BB238253-F355-4A5C-9AB8-1FA662EAD62F}"/>
-    <hyperlink ref="C28" r:id="rId21" xr:uid="{E5666281-7B26-4687-BB28-2199900A1080}"/>
-    <hyperlink ref="C30" r:id="rId22" xr:uid="{4C2BA448-D508-48B1-8ECE-E95B7EE8E697}"/>
-    <hyperlink ref="C31" r:id="rId23" xr:uid="{24C173A1-C8FC-446E-9A50-C963EA681A61}"/>
-    <hyperlink ref="C32" r:id="rId24" xr:uid="{FFDBBC53-FE5C-4074-8C48-F2A462425E55}"/>
-    <hyperlink ref="C34" r:id="rId25" xr:uid="{17C89D37-87D2-4E18-94CD-87AB8270DAEE}"/>
-    <hyperlink ref="C33" r:id="rId26" xr:uid="{66CAB1C1-B412-428E-A26F-76605F6594E4}"/>
-    <hyperlink ref="C37" r:id="rId27" xr:uid="{4F43174A-9092-4809-8B80-B1CE410EBA31}"/>
-    <hyperlink ref="C35" r:id="rId28" xr:uid="{0973DD32-FE77-49EC-A8A9-AAA722E88CAE}"/>
-    <hyperlink ref="C40" r:id="rId29" xr:uid="{9C54D993-F061-41F1-8F41-5541B78A6CF3}"/>
-    <hyperlink ref="C41" r:id="rId30" xr:uid="{68EF8942-6A9F-43A0-9B77-6C5BC0EF57E6}"/>
-    <hyperlink ref="C42" r:id="rId31" xr:uid="{ADE95A00-F8D2-4BEC-B973-525C7559C5B8}"/>
-    <hyperlink ref="C43" r:id="rId32" xr:uid="{54DF2E61-CD6E-46DE-AE5E-085F446DDB64}"/>
-    <hyperlink ref="C44" r:id="rId33" xr:uid="{57729F6F-298E-414A-85D8-A01E33AC8146}"/>
-    <hyperlink ref="C45" r:id="rId34" xr:uid="{CCAEA818-7FE4-4B74-81A4-E2174150131D}"/>
-    <hyperlink ref="C46" r:id="rId35" xr:uid="{3DCF6AE2-80CD-4326-8C4A-074CDC77B77D}"/>
-    <hyperlink ref="C47" r:id="rId36" xr:uid="{B16EC75D-1255-473E-BF41-4BEAFF1CB6C6}"/>
-    <hyperlink ref="C49" r:id="rId37" xr:uid="{216EABAD-1D44-4AC9-832A-4D8D02FC6022}"/>
-    <hyperlink ref="C51" r:id="rId38" location="&amp;&amp;D1XZLnCoo8Z0jHfshWy070zSzxdxFoNyojR7wLtsqBKXma2Biw1bPoNQ35FIlZ20OZFVPPWKm2NVjBEWid89Yl+5G1w9meYdtfsLaZvHbBvHz8jdUMP8SPwa2hhoYyoDM9h6+eiuYPSH9xhY49fqg35E6OgRxfcg1iJxtfHylJBLsGD1" xr:uid="{FC6108CD-C840-4B86-AA75-9AE510F8ABE0}"/>
+    <hyperlink ref="C14" r:id="rId7" xr:uid="{501D0F09-5707-41B2-9F84-0072E94D0FCE}"/>
+    <hyperlink ref="C15" r:id="rId8" xr:uid="{9D44CC03-093F-4F7E-8E5B-F0624B178431}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{15B65C99-090A-4014-8BC9-47AA25ABB5BD}"/>
+    <hyperlink ref="C17" r:id="rId10" xr:uid="{59ABBE2F-E96D-447A-A8BE-658D5BBCEBB9}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{52AB6CA7-2C51-483E-AB81-D8C456E36E4E}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{8CE5F8D3-2664-47BC-AC92-CC2AFB1F86E1}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{883FB522-98B0-4142-BAA1-CA9467FA04BB}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{668DB339-8157-4A7C-98BE-A963E1B2D647}"/>
+    <hyperlink ref="C21" r:id="rId15" xr:uid="{2EE67D5C-E95F-4BFA-8D94-1228F2F52D7D}"/>
+    <hyperlink ref="C22" r:id="rId16" xr:uid="{F8B3B7AF-6AE0-4640-B0B9-FFBE5B89099C}"/>
+    <hyperlink ref="C24" r:id="rId17" xr:uid="{41B67C76-9DC2-4056-ADBA-E03069095849}"/>
+    <hyperlink ref="C25" r:id="rId18" location="clear=1" xr:uid="{2BEEAB08-8AFB-4EE1-9899-E43718836604}"/>
+    <hyperlink ref="C26" r:id="rId19" xr:uid="{BB238253-F355-4A5C-9AB8-1FA662EAD62F}"/>
+    <hyperlink ref="C28" r:id="rId20" xr:uid="{E5666281-7B26-4687-BB28-2199900A1080}"/>
+    <hyperlink ref="C30" r:id="rId21" xr:uid="{4C2BA448-D508-48B1-8ECE-E95B7EE8E697}"/>
+    <hyperlink ref="C31" r:id="rId22" xr:uid="{24C173A1-C8FC-446E-9A50-C963EA681A61}"/>
+    <hyperlink ref="C32" r:id="rId23" xr:uid="{FFDBBC53-FE5C-4074-8C48-F2A462425E55}"/>
+    <hyperlink ref="C34" r:id="rId24" xr:uid="{17C89D37-87D2-4E18-94CD-87AB8270DAEE}"/>
+    <hyperlink ref="C33" r:id="rId25" xr:uid="{66CAB1C1-B412-428E-A26F-76605F6594E4}"/>
+    <hyperlink ref="C37" r:id="rId26" xr:uid="{4F43174A-9092-4809-8B80-B1CE410EBA31}"/>
+    <hyperlink ref="C35" r:id="rId27" xr:uid="{0973DD32-FE77-49EC-A8A9-AAA722E88CAE}"/>
+    <hyperlink ref="C40" r:id="rId28" xr:uid="{9C54D993-F061-41F1-8F41-5541B78A6CF3}"/>
+    <hyperlink ref="C41" r:id="rId29" xr:uid="{68EF8942-6A9F-43A0-9B77-6C5BC0EF57E6}"/>
+    <hyperlink ref="C42" r:id="rId30" xr:uid="{ADE95A00-F8D2-4BEC-B973-525C7559C5B8}"/>
+    <hyperlink ref="C43" r:id="rId31" xr:uid="{54DF2E61-CD6E-46DE-AE5E-085F446DDB64}"/>
+    <hyperlink ref="C44" r:id="rId32" xr:uid="{57729F6F-298E-414A-85D8-A01E33AC8146}"/>
+    <hyperlink ref="C45" r:id="rId33" xr:uid="{CCAEA818-7FE4-4B74-81A4-E2174150131D}"/>
+    <hyperlink ref="C46" r:id="rId34" xr:uid="{3DCF6AE2-80CD-4326-8C4A-074CDC77B77D}"/>
+    <hyperlink ref="C47" r:id="rId35" xr:uid="{B16EC75D-1255-473E-BF41-4BEAFF1CB6C6}"/>
+    <hyperlink ref="C49" r:id="rId36" xr:uid="{216EABAD-1D44-4AC9-832A-4D8D02FC6022}"/>
+    <hyperlink ref="C51" r:id="rId37" location="&amp;&amp;D1XZLnCoo8Z0jHfshWy070zSzxdxFoNyojR7wLtsqBKXma2Biw1bPoNQ35FIlZ20OZFVPPWKm2NVjBEWid89Yl+5G1w9meYdtfsLaZvHbBvHz8jdUMP8SPwa2hhoYyoDM9h6+eiuYPSH9xhY49fqg35E6OgRxfcg1iJxtfHylJBLsGD1" xr:uid="{FC6108CD-C840-4B86-AA75-9AE510F8ABE0}"/>
+    <hyperlink ref="C10" r:id="rId38" xr:uid="{8C6FF266-CAB6-4817-911C-DEA78521D44D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
26 states finished -- a few more added
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7355ddd88330403a/Documents/GitHub/sonny_side/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="372" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7297B84C-D7E6-43A6-8F09-73F6DF27575A}"/>
+  <xr:revisionPtr revIDLastSave="428" documentId="8_{704272EC-853A-440D-BE35-A05DE615BFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A695A6C9-7B50-47D4-BFC1-ADDE91DEADE6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="204">
   <si>
     <t>Alabama</t>
   </si>
@@ -393,9 +393,6 @@
     <t>Need spider - Page 1 of 2558, records 1 to 25 of 63936</t>
   </si>
   <si>
-    <t>48 records on csv ready to regex</t>
-  </si>
-  <si>
     <t>Has more button below table and each time it is clicked adds 10 records. Can we spider that?</t>
   </si>
   <si>
@@ -453,36 +450,15 @@
     <t>Using "full text" search found 2154 son and 3902 sons records. Removed emplty lines and dedup.</t>
   </si>
   <si>
-    <t>Annoying copy/paste generated 3 rows per company so prepared in xls. Had to search for daughter for active and inactive separately. 219 in CSV.</t>
-  </si>
-  <si>
-    <t>Capped at 500. Searched 4 times and rbind results for son &amp; sons vs. active/inactive. 2000 in CSV. Dedup in R.</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Very conservative since only got son coverage until letter d. Could redo and include starts with son but spider might be better</t>
-  </si>
-  <si>
-    <t>Search gives counts with exact match.</t>
-  </si>
-  <si>
-    <t>Spider needed if we want data in R</t>
-  </si>
-  <si>
-    <t>Need spider</t>
-  </si>
-  <si>
     <t>41 rows found and copy/pasted to csv</t>
   </si>
   <si>
     <t>?/41</t>
   </si>
   <si>
-    <t>keyword search of son gives error. Sons keyword search returns 1390 but really need spider</t>
-  </si>
-  <si>
     <t>120 contain daughter but need spider</t>
   </si>
   <si>
@@ -619,6 +595,57 @@
   </si>
   <si>
     <t>horrible excercse since links have to be hard coded. Use with CAUTION since only searches that start with daughter and son were allowed. Couldn't search for *daughter or *son unfortunately. Results are very partial.</t>
+  </si>
+  <si>
+    <t>Blocked cause I can't customize URL to rvest it</t>
+  </si>
+  <si>
+    <t>Don't see how to do this without many copy/paste</t>
+  </si>
+  <si>
+    <t>Can't customize URL for rvest and don't want to copy/paste hundreds of times</t>
+  </si>
+  <si>
+    <t>Blocked. URLs are customized but randomly so don't know how to iterate withouth having to copy paste all of them. Tried one of the links in R and failed anyway.</t>
+  </si>
+  <si>
+    <t>This is very odd and wouldn't use it and caveat heavily. Search results are limited to 250 results and there are 250 with daugther and 250 for son so ratio is 1 but who knows what else exists is Louisiana</t>
+  </si>
+  <si>
+    <t>Generated 8 links with all combos based on search parameters and then did spider. Deduped before extraction of word. Could have also used the csv I copy/pasted since results are not capped</t>
+  </si>
+  <si>
+    <t>Generated 8 links with all combos based on search parameters and then did spider. Deduped before extraction of word. Each search is capped at 500 so careful due to underrepresentation</t>
+  </si>
+  <si>
+    <t>son is underrepresented due to search cap so careful</t>
+  </si>
+  <si>
+    <t>752 anyword == son + 1166 anyword == sons</t>
+  </si>
+  <si>
+    <t>22 anyword == daughter + 143 anyword == daughters</t>
+  </si>
+  <si>
+    <t>Search gives counts with exact match so I just added it. But can't bring to R to do regex or dedup without spider and don't get a frinedly URL</t>
+  </si>
+  <si>
+    <t>439 found but format is horrible to copy and paste and need spider</t>
+  </si>
+  <si>
+    <t>Capped at 1854 but need to do regex and can't get url to spider</t>
+  </si>
+  <si>
+    <t>Horrible output format and can't customize URL for rvest</t>
+  </si>
+  <si>
+    <t>keyword search of son gives error. Sons keyword search returns 1390 but really need spider to get to r to do regex</t>
+  </si>
+  <si>
+    <t>Can't get URL to rvest, help!</t>
+  </si>
+  <si>
+    <t>Blocked cause can't generate url to rvest. Perhaps many copy/pastes if not</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,10 +1088,10 @@
         <v>106</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1101,7 +1128,7 @@
         <v>114</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1124,7 +1151,7 @@
         <v>115</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1147,7 +1174,7 @@
         <v>112</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1181,10 +1208,10 @@
         <v>113</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1198,13 +1225,13 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G8" s="5">
         <f>875/43</f>
@@ -1222,20 +1249,20 @@
         <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>116</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="G9" s="5">
         <f>24/33</f>
         <v>0.72727272727272729</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -1249,23 +1276,23 @@
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="G10" s="5">
         <f>729/176</f>
         <v>4.1420454545454541</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1276,13 +1303,16 @@
         <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>118</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1330,7 +1360,10 @@
         <v>119</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1344,16 +1377,19 @@
         <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1364,13 +1400,16 @@
         <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>124</v>
+      <c r="H16" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1384,13 +1423,13 @@
         <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="G17" s="5">
         <f>75/14</f>
@@ -1408,20 +1447,20 @@
         <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G18" s="5">
         <f>66/16</f>
         <v>4.125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1432,13 +1471,20 @@
         <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>132</v>
+      <c r="G19" s="5">
+        <f>250/250</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1452,13 +1498,13 @@
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G20" s="6">
         <f>45/52</f>
@@ -1476,13 +1522,13 @@
         <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="G21" s="5">
         <f>128/82</f>
@@ -1500,13 +1546,13 @@
         <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G22" s="5">
         <f>5979/147</f>
@@ -1527,7 +1573,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1538,23 +1584,23 @@
         <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>139</v>
+        <v>192</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="G24" s="5">
-        <f>222/212</f>
-        <v>1.0471698113207548</v>
+        <f>392/213</f>
+        <v>1.84037558685446</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1565,23 +1611,23 @@
         <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="G25" s="5">
-        <f>752/22</f>
-        <v>34.18181818181818</v>
+        <f>(752+1166)/(22+143)</f>
+        <v>11.624242424242425</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1592,13 +1638,16 @@
         <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>145</v>
+        <v>198</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>145</v>
+        <v>199</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1626,16 +1675,16 @@
         <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1663,16 +1712,19 @@
         <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1683,16 +1735,19 @@
         <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1706,10 +1761,10 @@
         <v>107</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1726,10 +1781,10 @@
         <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1746,10 +1801,10 @@
         <v>107</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1766,10 +1821,10 @@
         <v>110</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1800,10 +1855,10 @@
         <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1845,13 +1900,13 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G40" s="5">
         <f>206/12</f>
@@ -1869,20 +1924,20 @@
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G41" s="5">
         <f>(27222*9/60)/59</f>
         <v>69.208474576271186</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1896,13 +1951,13 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G42" s="5">
         <f>129/11</f>
@@ -1923,10 +1978,10 @@
         <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1943,10 +1998,10 @@
         <v>110</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1963,10 +2018,10 @@
         <v>107</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1983,10 +2038,10 @@
         <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2003,10 +2058,10 @@
         <v>107</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2037,10 +2092,10 @@
         <v>107</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2071,17 +2126,17 @@
         <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}">
     <filterColumn colId="0">
       <filters>
-        <filter val="10"/>
+        <filter val="31"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">

</xml_diff>

<commit_message>
5 more states by Walter on 12/28
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sons_and_daughters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EF658C-4051-420D-A706-CD697F3E4846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{78EF658C-4051-420D-A706-CD697F3E4846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E0F9095-CA74-4992-8240-33B137A9DCE5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="207">
   <si>
     <t>Alabama</t>
   </si>
@@ -359,9 +357,6 @@
     <t>Son search</t>
   </si>
   <si>
-    <t>23 companies with daughter or daughters on it. Still need to do a regex</t>
-  </si>
-  <si>
     <t>163 companies in 9 pages - need spider</t>
   </si>
   <si>
@@ -371,36 +366,15 @@
     <t xml:space="preserve">91 records found, copied into csv. </t>
   </si>
   <si>
-    <t>14240 records found in pages of 250 - need spider</t>
-  </si>
-  <si>
     <t>Need spider - Found 309 matching record(s).  Viewing page 1 of 16.</t>
   </si>
   <si>
-    <t>Results capped at 2,000 and hard to copy/paste since only shows 20 per page. Need spider.</t>
-  </si>
-  <si>
     <t>Your Search Criteria returns 43783 results which is more than 500 results. Need to figure out how to get 500 son and then spider</t>
   </si>
   <si>
     <t>Found 33 and are in csv ready for regex</t>
   </si>
   <si>
-    <t xml:space="preserve">Need spider - Page 2 of 21, records 26 to 50 of 513 </t>
-  </si>
-  <si>
-    <t>Need spider - Page 1 of 2558, records 1 to 25 of 63936</t>
-  </si>
-  <si>
-    <t>Has more button below table and each time it is clicked adds 10 records. Can we spider that?</t>
-  </si>
-  <si>
-    <t>Could copy/paste but spider would be better - Page 1 of 8, records 1 to 25 of 199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need spider - Page 1 of 1440, records 1 to 25 of 35979  </t>
-  </si>
-  <si>
     <t>Could copy/paste but spider would be better - Results 1 - 25 of 74</t>
   </si>
   <si>
@@ -509,9 +483,6 @@
     <t>Was able to search "contains" and got 141. Copy pasted ok to csv</t>
   </si>
   <si>
-    <t>Caps at 500 and displays 100 per page so need spider. Could do multiple searches to increase n results</t>
-  </si>
-  <si>
     <t>daughter search would yield 221 but doesn't show. Daughters show 152 results.</t>
   </si>
   <si>
@@ -527,9 +498,6 @@
     <t>65 rows copy pasted to csv</t>
   </si>
   <si>
-    <t>7393 results in 296 pages contain son, need spider</t>
-  </si>
-  <si>
     <t>Page 1 of 12, records 1 to 25 of 278 -- need spider</t>
   </si>
   <si>
@@ -545,15 +513,9 @@
     <t>Found 679 with son* and 2954 with *son. Was able to relatively easy copy/paste in xls and then dedup in R</t>
   </si>
   <si>
-    <t>Can't get rvest to run even with Gaurav generated URL</t>
-  </si>
-  <si>
     <t>Need to figure out how to create customized URL to use rvest - help!</t>
   </si>
   <si>
-    <t>Could copy/paste since pages are 250 long but better if I can create customized url to rvest</t>
-  </si>
-  <si>
     <t>Only works with searches of 500 or less results so need to trim/hack. Results in 30 pages so need spider</t>
   </si>
   <si>
@@ -575,15 +537,6 @@
     <t>horrible excercse since links have to be hard coded. Use with CAUTION since only searches that start with daughter and son were allowed. Couldn't search for *daughter or *son unfortunately. Results are very partial.</t>
   </si>
   <si>
-    <t>Blocked cause I can't customize URL to rvest it</t>
-  </si>
-  <si>
-    <t>Don't see how to do this without many copy/paste</t>
-  </si>
-  <si>
-    <t>Can't customize URL for rvest and don't want to copy/paste hundreds of times</t>
-  </si>
-  <si>
     <t>Blocked. URLs are customized but randomly so don't know how to iterate withouth having to copy paste all of them. Tried one of the links in R and failed anyway.</t>
   </si>
   <si>
@@ -650,18 +603,12 @@
     <t>Can't generate URL to rvest. Could copy paste but would be long.</t>
   </si>
   <si>
-    <t>Can't generate URL to rvest. Could copy paste but would be long like 20x.</t>
-  </si>
-  <si>
     <t>I think it doesn't show if 200+? Rows. What we do?</t>
   </si>
   <si>
     <t>URL is not fully customizable to rvest so blocked. Copy/paste could work but it is very odd and would need to do it like 15x.</t>
   </si>
   <si>
-    <t>Can't get URL to rvest, help! Copy/paste would kill me</t>
-  </si>
-  <si>
     <t>Your Search Criteria returns 29121 results which is more than 500 results. Can show all results but copy/paste would be horrible</t>
   </si>
   <si>
@@ -678,6 +625,36 @@
   </si>
   <si>
     <t>Can't be Done</t>
+  </si>
+  <si>
+    <t>I copy pasted and did regex</t>
+  </si>
+  <si>
+    <t>Gaurav grabbed data with selenium. I did estimates and cleaning in R</t>
+  </si>
+  <si>
+    <t>Gaurav pulled with selenium and I calculated</t>
+  </si>
+  <si>
+    <t>Need Gaurav's help</t>
+  </si>
+  <si>
+    <t>Gaurav did selenium for son only, so need to run for daughter</t>
+  </si>
+  <si>
+    <t>Need help to run with Selenium</t>
+  </si>
+  <si>
+    <t>I copy pasted from 8 pages</t>
+  </si>
+  <si>
+    <t>Problematic search since capped at 500. Searched multiple times for son/sons and start/contains mix to maximize n. But son is severely underrepresented</t>
+  </si>
+  <si>
+    <t>Son is severely underrepresented so caveat this estimate.</t>
+  </si>
+  <si>
+    <t>Gaurav pulled with rvest loop and I calculated</t>
   </si>
 </sst>
 </file>
@@ -1082,11 +1059,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE50C96B-AE9B-4FF9-A241-178704DDBFF3}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,13 +1100,13 @@
         <v>106</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1142,7 +1120,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1153,19 +1131,20 @@
         <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="G3" s="5">
+        <f>246/22</f>
+        <v>11.181818181818182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1176,19 +1155,19 @@
         <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1199,19 +1178,20 @@
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G5" s="5">
+        <f>1482/87</f>
+        <v>17.03448275862069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1225,7 +1205,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1236,19 +1216,19 @@
         <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1259,20 +1239,20 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G8" s="5">
         <f>875/43</f>
         <v>20.348837209302324</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1283,23 +1263,23 @@
         <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="G9" s="5">
         <f>24/33</f>
         <v>0.72727272727272729</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1310,23 +1290,23 @@
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="G10" s="5">
         <f>729/176</f>
         <v>4.1420454545454541</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1337,19 +1317,16 @@
         <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1363,7 +1340,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1388,19 +1365,16 @@
         <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>118</v>
+        <v>201</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1411,16 +1385,17 @@
         <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>119</v>
+        <v>203</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
+      </c>
+      <c r="G15" s="5">
+        <f>4928/195</f>
+        <v>25.271794871794871</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1434,19 +1409,19 @@
         <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1457,20 +1432,20 @@
         <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="G17" s="5">
         <f>75/14</f>
         <v>5.3571428571428568</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1481,20 +1456,20 @@
         <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G18" s="5">
         <f>66/16</f>
         <v>4.125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1505,23 +1480,23 @@
         <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G19" s="5">
         <f>250/250</f>
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1532,20 +1507,20 @@
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G20" s="6">
         <f>45/52</f>
         <v>0.86538461538461542</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1556,20 +1531,20 @@
         <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G21" s="5">
         <f>128/82</f>
         <v>1.5609756097560976</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1580,20 +1555,20 @@
         <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G22" s="5">
         <f>5979/147</f>
         <v>40.673469387755105</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1607,7 +1582,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1618,23 +1593,23 @@
         <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="G24" s="5">
         <f>392/213</f>
         <v>1.84037558685446</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1645,20 +1620,20 @@
         <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G25" s="5">
         <f>(752+1166)/(22+143)</f>
         <v>11.624242424242425</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1672,19 +1647,19 @@
         <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1709,19 +1684,19 @@
         <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1746,16 +1721,16 @@
         <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1769,16 +1744,16 @@
         <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1792,19 +1767,19 @@
         <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1815,20 +1790,20 @@
         <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="G33" s="5">
         <f>1190/745</f>
         <v>1.5973154362416107</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1842,19 +1817,19 @@
         <v>63</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1865,23 +1840,23 @@
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G35" s="5">
         <f>605/23</f>
         <v>26.304347826086957</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1906,19 +1881,19 @@
         <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1932,7 +1907,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1946,7 +1921,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1957,20 +1932,20 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G40" s="5">
         <f>206/12</f>
         <v>17.166666666666668</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1981,23 +1956,23 @@
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G41" s="5">
         <f>(27222*9/60)/59</f>
         <v>69.208474576271186</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2008,20 +1983,20 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G42" s="5">
         <f>129/11</f>
         <v>11.727272727272727</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2032,19 +2007,23 @@
         <v>85</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>157</v>
+        <v>204</v>
+      </c>
+      <c r="G43" s="5">
+        <f>203/132</f>
+        <v>1.5378787878787878</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2055,16 +2034,16 @@
         <v>87</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2078,19 +2057,19 @@
         <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2101,16 +2080,17 @@
         <v>91</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
+      </c>
+      <c r="G46" s="5">
+        <f>1361/63</f>
+        <v>21.603174603174605</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2124,19 +2104,19 @@
         <v>93</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2161,19 +2141,19 @@
         <v>97</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2187,7 +2167,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2198,24 +2178,31 @@
         <v>101</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="G51" s="5">
         <f>238/21</f>
         <v>11.333333333333334</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}"/>
+  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Blocked"/>
+        <filter val="Need Gaurav's help"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{57FE75D0-032C-4AC1-83C8-CCA0DEF7DD1E}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{DAAD63D8-7315-40FF-A6E5-CCD3001C4F5B}"/>

</xml_diff>

<commit_message>
A few more added - we are at 37 done
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{78EF658C-4051-420D-A706-CD697F3E4846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E0F9095-CA74-4992-8240-33B137A9DCE5}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{78EF658C-4051-420D-A706-CD697F3E4846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A6E90D91-41A3-4BAF-913D-C743076BB74B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="209">
   <si>
     <t>Alabama</t>
   </si>
@@ -441,9 +441,6 @@
     <t>74 contain daughter, need spider</t>
   </si>
   <si>
-    <t>Caps at 500, need spider</t>
-  </si>
-  <si>
     <t>52 contain daughter, need spider</t>
   </si>
   <si>
@@ -489,12 +486,6 @@
     <t>son would yield 4,740 but doesn't show. Sons would yiled 275 but doesn't show</t>
   </si>
   <si>
-    <t>son yields 690 results in 14 pages. Need spider</t>
-  </si>
-  <si>
-    <t>daughter yields 17 results but copy/paste not working. Maybe spider?</t>
-  </si>
-  <si>
     <t>65 rows copy pasted to csv</t>
   </si>
   <si>
@@ -537,9 +528,6 @@
     <t>horrible excercse since links have to be hard coded. Use with CAUTION since only searches that start with daughter and son were allowed. Couldn't search for *daughter or *son unfortunately. Results are very partial.</t>
   </si>
   <si>
-    <t>Blocked. URLs are customized but randomly so don't know how to iterate withouth having to copy paste all of them. Tried one of the links in R and failed anyway.</t>
-  </si>
-  <si>
     <t>This is very odd and wouldn't use it and caveat heavily. Search results are limited to 250 results and there are 250 with daugther and 250 for son so ratio is 1 but who knows what else exists is Louisiana</t>
   </si>
   <si>
@@ -567,18 +555,12 @@
     <t>Capped at 1854 but need to do regex and can't get url to spider</t>
   </si>
   <si>
-    <t>Horrible output format and can't customize URL for rvest</t>
-  </si>
-  <si>
     <t>keyword search of son gives error. Sons keyword search returns 1390 but really need spider to get to r to do regex</t>
   </si>
   <si>
     <t>Can't get URL to rvest, help!</t>
   </si>
   <si>
-    <t>Blocked cause can't generate url to rvest. Perhaps many copy/pastes if not</t>
-  </si>
-  <si>
     <t>Has I'm not robot captcha. No friendly url to rvest is generated so what we do? Total No. of Records: 7877 Page 1 of 788</t>
   </si>
   <si>
@@ -606,9 +588,6 @@
     <t>I think it doesn't show if 200+? Rows. What we do?</t>
   </si>
   <si>
-    <t>URL is not fully customizable to rvest so blocked. Copy/paste could work but it is very odd and would need to do it like 15x.</t>
-  </si>
-  <si>
     <t>Your Search Criteria returns 29121 results which is more than 500 results. Can show all results but copy/paste would be horrible</t>
   </si>
   <si>
@@ -636,15 +615,6 @@
     <t>Gaurav pulled with selenium and I calculated</t>
   </si>
   <si>
-    <t>Need Gaurav's help</t>
-  </si>
-  <si>
-    <t>Gaurav did selenium for son only, so need to run for daughter</t>
-  </si>
-  <si>
-    <t>Need help to run with Selenium</t>
-  </si>
-  <si>
     <t>I copy pasted from 8 pages</t>
   </si>
   <si>
@@ -655,6 +625,42 @@
   </si>
   <si>
     <t>Gaurav pulled with rvest loop and I calculated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaurav pulled with selenium </t>
+  </si>
+  <si>
+    <t>Walter copy/pasted 516 rows from 21 screens</t>
+  </si>
+  <si>
+    <t>Walter copy/pasted from search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaurav did selenium </t>
+  </si>
+  <si>
+    <t>Blocked. URLs are customized but randomly so don't know how to iterate withouth having to copy paste all of them. Tried one of the links in R and failed anyway. Walter can do it with lots of copy/pastes if there is not another option?</t>
+  </si>
+  <si>
+    <t>Horrible output format and can't customize URL for rvest. @Gaurav, can you scrap or I can try and do many copy/pastes?</t>
+  </si>
+  <si>
+    <t>Keep getting error, try later.</t>
+  </si>
+  <si>
+    <t>Caps at 500, need spider cause shows only 10 per page</t>
+  </si>
+  <si>
+    <t>Blocked cause can't generate url to rvest. Copy/pastse is last resort</t>
+  </si>
+  <si>
+    <t>Copy pasted but it's messy cause combines all attributes but ok for our work</t>
+  </si>
+  <si>
+    <t>690 for son* copy pasted. For *son I need spider and I can't get URL link like Arkansas as Gaurav suggested</t>
+  </si>
+  <si>
+    <t>son is EXTREMELY underrepresented. If we want more accurate # I need help from Gaurav for son spider. But this ratio makes point and extremely conservative</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1070,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,17 +1140,17 @@
         <v>118</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G3" s="5">
         <f>246/22</f>
         <v>11.181818181818182</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>107</v>
@@ -1164,7 +1170,7 @@
         <v>111</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1184,7 +1190,7 @@
         <v>109</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="G5" s="5">
         <f>1482/87</f>
@@ -1205,7 +1211,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1216,16 +1222,16 @@
         <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>110</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1242,10 +1248,10 @@
         <v>118</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G8" s="5">
         <f>875/43</f>
@@ -1269,14 +1275,14 @@
         <v>112</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G9" s="5">
         <f>24/33</f>
         <v>0.72727272727272729</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -1293,20 +1299,20 @@
         <v>118</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G10" s="5">
         <f>729/176</f>
         <v>4.1420454545454541</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1317,13 +1323,17 @@
         <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
+      </c>
+      <c r="G11" s="5">
+        <f>6002/497</f>
+        <v>12.076458752515091</v>
       </c>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1354,7 +1364,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1365,13 +1375,17 @@
         <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>201</v>
+      <c r="G14" s="5">
+        <f>2324/48</f>
+        <v>48.416666666666664</v>
       </c>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1388,17 +1402,17 @@
         <v>118</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G15" s="5">
         <f>4928/195</f>
         <v>25.271794871794871</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1418,7 +1432,7 @@
         <v>114</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1493,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1596,17 +1610,17 @@
         <v>118</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G24" s="5">
         <f>392/213</f>
         <v>1.84037558685446</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1623,17 +1637,17 @@
         <v>118</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G25" s="5">
         <f>(752+1166)/(22+143)</f>
         <v>11.624242424242425</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1650,13 +1664,13 @@
         <v>108</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1690,10 +1704,13 @@
         <v>130</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>131</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1730,10 +1747,10 @@
         <v>133</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1750,10 +1767,10 @@
         <v>134</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1770,13 +1787,13 @@
         <v>108</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="H32" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -1793,17 +1810,17 @@
         <v>118</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G33" s="5">
         <f>1190/745</f>
         <v>1.5973154362416107</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1820,13 +1837,13 @@
         <v>108</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1843,17 +1860,17 @@
         <v>118</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G35" s="5">
         <f>605/23</f>
         <v>26.304347826086957</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1884,13 +1901,13 @@
         <v>108</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="H37" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1935,10 +1952,10 @@
         <v>118</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G40" s="5">
         <f>206/12</f>
@@ -1959,17 +1976,17 @@
         <v>118</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="G41" s="5">
         <f>(27222*9/60)/59</f>
         <v>69.208474576271186</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1986,10 +2003,10 @@
         <v>118</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G42" s="5">
         <f>129/11</f>
@@ -2010,20 +2027,20 @@
         <v>118</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="G43" s="5">
         <f>203/132</f>
         <v>1.5378787878787878</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2034,19 +2051,19 @@
         <v>87</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2057,16 +2074,20 @@
         <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>152</v>
+        <v>206</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>151</v>
+        <v>207</v>
+      </c>
+      <c r="G45" s="5">
+        <f>81/16</f>
+        <v>5.0625</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2083,10 +2104,10 @@
         <v>118</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G46" s="5">
         <f>1361/63</f>
@@ -2107,13 +2128,13 @@
         <v>108</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2144,13 +2165,13 @@
         <v>108</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2181,17 +2202,17 @@
         <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G51" s="5">
         <f>238/21</f>
         <v>11.333333333333334</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2199,7 +2220,7 @@
     <filterColumn colId="3">
       <filters>
         <filter val="Blocked"/>
-        <filter val="Need Gaurav's help"/>
+        <filter val="Can't be Done"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
nh wv nj are done!
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{93A9F197-CF9F-4AC5-859A-86253AC9A13C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{188E6F21-12CC-4748-AB86-FF2C1D21AD36}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{93A9F197-CF9F-4AC5-859A-86253AC9A13C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{127B0F2C-3CFB-4847-9378-5DF9D0AE2491}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="205">
   <si>
     <t>Alabama</t>
   </si>
@@ -432,9 +432,6 @@
     <t>?/41</t>
   </si>
   <si>
-    <t>74 contain daughter, need spider</t>
-  </si>
-  <si>
     <t>52 contain daughter, need spider</t>
   </si>
   <si>
@@ -486,12 +483,6 @@
     <t>Page 1 of 12, records 1 to 25 of 278 -- need spider</t>
   </si>
   <si>
-    <t>76 results in 8 pages, spider would be best</t>
-  </si>
-  <si>
-    <t>shows up to 1000 results in pages of 10 - ouch. Needs spider</t>
-  </si>
-  <si>
     <t>Found 27 with DAUGHTER* &amp; 19 with *DAUGHTER. Copied easily to CSV</t>
   </si>
   <si>
@@ -585,9 +576,6 @@
     <t xml:space="preserve">Can't get URL to rvest and copy/paste would be too much. </t>
   </si>
   <si>
-    <t>URL pattern is ood. Rvest works almost but need pattern to loop.</t>
-  </si>
-  <si>
     <t>Was able to download the full DB in a friendly way. Had to do some sorting and cleaning in excel cause R was freaking so used edited version.</t>
   </si>
   <si>
@@ -639,12 +627,6 @@
     <t>Keep getting error, try later.</t>
   </si>
   <si>
-    <t>Caps at 500, need spider cause shows only 10 per page</t>
-  </si>
-  <si>
-    <t>Blocked cause can't generate url to rvest. Copy/pastse is last resort</t>
-  </si>
-  <si>
     <t>Copy pasted but it's messy cause combines all attributes but ok for our work</t>
   </si>
   <si>
@@ -655,6 +637,18 @@
   </si>
   <si>
     <t>I copy pasted</t>
+  </si>
+  <si>
+    <t>Super conservative estimate for son cause search results truncated at 1000</t>
+  </si>
+  <si>
+    <t>Was able to copy/paste all with daughter</t>
+  </si>
+  <si>
+    <t>Copy pasted but results truncated at 500 so combined son and sons search to increase n and then deduped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super conservative estimate for son cause search results truncated at 500 on search. </t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1057,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,17 +1128,17 @@
         <v>118</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G3" s="5">
         <f>246/22</f>
         <v>11.181818181818182</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1155,7 +1149,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>107</v>
@@ -1164,7 +1158,7 @@
         <v>111</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1184,7 +1178,7 @@
         <v>109</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G5" s="5">
         <f>1482/87</f>
@@ -1205,7 +1199,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1216,16 +1210,16 @@
         <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>110</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1242,10 +1236,10 @@
         <v>118</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G8" s="5">
         <f>875/43</f>
@@ -1269,14 +1263,14 @@
         <v>112</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G9" s="5">
         <f>24/33</f>
         <v>0.72727272727272729</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -1293,17 +1287,17 @@
         <v>118</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G10" s="5">
         <f>729/176</f>
         <v>4.1420454545454541</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1320,10 +1314,10 @@
         <v>118</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G11" s="5">
         <f>6002/497</f>
@@ -1372,10 +1366,10 @@
         <v>118</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G14" s="5">
         <f>2324/48</f>
@@ -1396,10 +1390,10 @@
         <v>118</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G15" s="5">
         <f>4928/195</f>
@@ -1426,7 +1420,7 @@
         <v>114</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1501,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1604,17 +1598,17 @@
         <v>118</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G24" s="5">
         <f>392/213</f>
         <v>1.84037558685446</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1631,17 +1625,17 @@
         <v>118</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G25" s="5">
         <f>(752+1166)/(22+143)</f>
         <v>11.624242424242425</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1658,13 +1652,13 @@
         <v>108</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1698,13 +1692,13 @@
         <v>130</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>131</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1721,7 +1715,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1735,17 +1729,17 @@
         <v>118</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G30" s="5">
         <f>3203/119</f>
         <v>26.915966386554622</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1756,16 +1750,20 @@
         <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
+      </c>
+      <c r="G31" s="5">
+        <f>173/73</f>
+        <v>2.3698630136986303</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1782,13 +1780,13 @@
         <v>108</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="H32" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -1805,17 +1803,17 @@
         <v>118</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G33" s="5">
         <f>1190/745</f>
         <v>1.5973154362416107</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1832,13 +1830,13 @@
         <v>108</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1855,17 +1853,17 @@
         <v>118</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G35" s="5">
         <f>605/23</f>
         <v>26.304347826086957</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1896,13 +1894,13 @@
         <v>108</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="H37" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1947,10 +1945,10 @@
         <v>118</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G40" s="5">
         <f>206/12</f>
@@ -1971,17 +1969,17 @@
         <v>118</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="G41" s="5">
         <f>(27222*9/60)/59</f>
         <v>69.208474576271186</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1998,10 +1996,10 @@
         <v>118</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G42" s="5">
         <f>129/11</f>
@@ -2022,20 +2020,20 @@
         <v>118</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G43" s="5">
         <f>203/132</f>
         <v>1.5378787878787878</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2046,16 +2044,16 @@
         <v>87</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2072,17 +2070,17 @@
         <v>118</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G45" s="5">
         <f>81/16</f>
         <v>5.0625</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2099,10 +2097,10 @@
         <v>118</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G46" s="5">
         <f>1361/63</f>
@@ -2123,13 +2121,13 @@
         <v>108</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2146,7 +2144,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2160,13 +2158,17 @@
         <v>118</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>151</v>
+        <v>193</v>
+      </c>
+      <c r="G49" s="5">
+        <f>128/72</f>
+        <v>1.7777777777777777</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2197,17 +2199,17 @@
         <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G51" s="5">
         <f>238/21</f>
         <v>11.333333333333334</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2215,7 +2217,6 @@
     <filterColumn colId="3">
       <filters>
         <filter val="Blocked"/>
-        <filter val="Can't be Done"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added son and daughter columns and Gauravs numbers from readme.md
</commit_message>
<xml_diff>
--- a/states-work-tracker.xlsx
+++ b/states-work-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wguil\OneDrive\Documents\GitHub\sonny_side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{93A9F197-CF9F-4AC5-859A-86253AC9A13C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{127B0F2C-3CFB-4847-9378-5DF9D0AE2491}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:1_{93A9F197-CF9F-4AC5-859A-86253AC9A13C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{946E977C-A6B6-4EEF-AD68-2DB7A9CE5482}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F0483F49-7B73-4DC7-9674-D3667AC7232E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="216">
   <si>
     <t>Alabama</t>
   </si>
@@ -351,12 +351,6 @@
     <t>Gaurav did</t>
   </si>
   <si>
-    <t>Daughter search</t>
-  </si>
-  <si>
-    <t>Son search</t>
-  </si>
-  <si>
     <t>163 companies in 9 pages - need spider</t>
   </si>
   <si>
@@ -387,9 +381,6 @@
     <t>results capped at 400 so searched for son and sons and rbind - 450-ish (need to dedup before regex)</t>
   </si>
   <si>
-    <t>Conservative Estimate</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -429,9 +420,6 @@
     <t>41 rows found and copy/pasted to csv</t>
   </si>
   <si>
-    <t>?/41</t>
-  </si>
-  <si>
     <t>52 contain daughter, need spider</t>
   </si>
   <si>
@@ -501,9 +489,6 @@
     <t>Only gives 50 results per search so I got 100 (son &amp; sons) search. I can't hack more results</t>
   </si>
   <si>
-    <t>CAUTION: Use carefuly since son is super under represented. I Just can't get more than 50 searches of son</t>
-  </si>
-  <si>
     <t>9 links parsed with spider</t>
   </si>
   <si>
@@ -624,9 +609,6 @@
     <t>Horrible output format and can't customize URL for rvest. @Gaurav, can you scrap or I can try and do many copy/pastes?</t>
   </si>
   <si>
-    <t>Keep getting error, try later.</t>
-  </si>
-  <si>
     <t>Copy pasted but it's messy cause combines all attributes but ok for our work</t>
   </si>
   <si>
@@ -649,6 +631,59 @@
   </si>
   <si>
     <t xml:space="preserve">Super conservative estimate for son cause search results truncated at 500 on search. </t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
+    <t>daughter</t>
+  </si>
+  <si>
+    <t>Daughter_search</t>
+  </si>
+  <si>
+    <t>Son_search</t>
+  </si>
+  <si>
+    <t>Conservative_ Estimate</t>
+  </si>
+  <si>
+    <t>AL returns at max. 1000 results. Results for son(s) are over a 1000. But when you apply regex to the 1,000, 884 come up as true positive. So the most conservative son:daughter ratio is 4.</t>
+  </si>
+  <si>
+    <t>CA returns a max. of 500 results. But it gives you total results (3609 vs. 150). We download the 500 results for son(s) and apply the regex. 499 come up as true positive. So the most conservative son:daughter ratio is 24.</t>
+  </si>
+  <si>
+    <t>CAUTION: Use carefuly since son is super under represented. I Just can't get more than 50 searches of son. 24/33 was result. Don't use cause misleading</t>
+  </si>
+  <si>
+    <t>HI returns a max. of 300 results. But it gives you total results (10,641 vs. 88). We download the 300 results for son(s) and apply the regex. 41 come up as true positive. So adjusted estimate = (41/300)*10,641 = 1454. The most conservative son:daughter ratio is 17.</t>
+  </si>
+  <si>
+    <t>regex used: .*_son(s)_.* and .*_daughter(s)_.*</t>
+  </si>
+  <si>
+    <t>45/52 was ratio but it's wrong since son is underrepresented</t>
+  </si>
+  <si>
+    <t>MT provides all the search results and we run a regex to narrow down to cases where son(s) is a separate word. A brief glimpse suggests all of the results are legitimate, of the variety X and Son(s) etc. There the ratio between business names with the word son and daughter is about 4.</t>
+  </si>
+  <si>
+    <t>Keep getting error, try later. Son search gives error due to count</t>
+  </si>
+  <si>
+    <t>1000+ so son under rep. OR doesn't return more than 1,000 results. Results for son are over a 1000. But when you apply regex to the 1,000, 985 come up as true positive. So the most conservative son:daughter ratio is 4.</t>
+  </si>
+  <si>
+    <t>doesn't seem to allow for exhaustive search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WA returns all the results and after applying the regex, we get 2,424 results for son(s). This means a ratio of 15.
+</t>
+  </si>
+  <si>
+    <t>Searches for "son" as a separate word.
+Had to do multiple searches---breaking by time---for son as results &gt; 500</t>
   </si>
 </sst>
 </file>
@@ -657,7 +692,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -724,18 +759,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1053,12 +1088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE50C96B-AE9B-4FF9-A241-178704DDBFF3}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,14 +1101,14 @@
     <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="71.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="18.140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="64.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -1088,19 +1122,25 @@
         <v>103</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1113,8 +1153,21 @@
       <c r="D2" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="7">
+        <f>H2/I2</f>
+        <v>7.0158730158730158</v>
+      </c>
+      <c r="H2" s="7">
+        <v>884</v>
+      </c>
+      <c r="I2" s="7">
+        <v>126</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1125,20 +1178,26 @@
         <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G3" s="5">
+        <v>179</v>
+      </c>
+      <c r="G3" s="7">
         <f>246/22</f>
         <v>11.181818181818182</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="7">
+        <v>246</v>
+      </c>
+      <c r="I3" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1149,19 +1208,19 @@
         <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1172,20 +1231,26 @@
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="5">
-        <f>1482/87</f>
+        <v>184</v>
+      </c>
+      <c r="G5" s="7">
+        <f>H5/I5</f>
         <v>17.03448275862069</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="7">
+        <v>1482</v>
+      </c>
+      <c r="I5" s="7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1198,8 +1263,21 @@
       <c r="D6" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="7">
+        <f>H6/I6</f>
+        <v>24.06</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3609</v>
+      </c>
+      <c r="I6" s="7">
+        <v>150</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1210,19 +1288,19 @@
         <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1233,20 +1311,26 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="5">
-        <f>875/43</f>
+        <v>146</v>
+      </c>
+      <c r="G8" s="7">
+        <f>H8/I8</f>
         <v>20.348837209302324</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="7">
+        <v>875</v>
+      </c>
+      <c r="I8" s="7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1257,50 +1341,52 @@
         <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G9" s="5">
-        <f>24/33</f>
-        <v>0.72727272727272729</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="5">
-        <f>729/176</f>
+        <v>152</v>
+      </c>
+      <c r="G10" s="7">
+        <f>H10/I10</f>
         <v>4.1420454545454541</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="7">
+        <v>729</v>
+      </c>
+      <c r="I10" s="7">
+        <v>176</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1311,20 +1397,26 @@
         <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G11" s="5">
-        <f>6002/497</f>
+        <v>185</v>
+      </c>
+      <c r="G11" s="7">
+        <f>H11/I11</f>
         <v>12.076458752515091</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="7">
+        <v>6002</v>
+      </c>
+      <c r="I11" s="7">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1337,8 +1429,21 @@
       <c r="D12" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="7">
+        <f>H12/I12</f>
+        <v>16.522727272727273</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1454</v>
+      </c>
+      <c r="I12" s="7">
+        <v>88</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1351,8 +1456,21 @@
       <c r="D13" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="7">
+        <f>H13/I13</f>
+        <v>1.5384615384615385</v>
+      </c>
+      <c r="H13" s="7">
+        <v>60</v>
+      </c>
+      <c r="I13" s="7">
+        <v>39</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1363,20 +1481,26 @@
         <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G14" s="5">
-        <f>2324/48</f>
+        <v>188</v>
+      </c>
+      <c r="G14" s="7">
+        <f>H14/I14</f>
         <v>48.416666666666664</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="7">
+        <v>2324</v>
+      </c>
+      <c r="I14" s="7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1387,20 +1511,26 @@
         <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" s="5">
-        <f>4928/195</f>
+        <v>180</v>
+      </c>
+      <c r="G15" s="7">
+        <f>H15/I15</f>
         <v>25.271794871794871</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H15" s="7">
+        <v>4928</v>
+      </c>
+      <c r="I15" s="7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1411,19 +1541,19 @@
         <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1434,20 +1564,26 @@
         <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" s="5">
-        <f>75/14</f>
+        <v>114</v>
+      </c>
+      <c r="G17" s="7">
+        <f>H17/I17</f>
         <v>5.3571428571428568</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="7">
+        <v>75</v>
+      </c>
+      <c r="I17" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1458,20 +1594,26 @@
         <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="5">
-        <f>66/16</f>
+        <v>117</v>
+      </c>
+      <c r="G18" s="7">
+        <f>H18/I18</f>
         <v>4.125</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="7">
+        <v>66</v>
+      </c>
+      <c r="I18" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1482,23 +1624,19 @@
         <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G19" s="5">
-        <f>250/250</f>
-        <v>1</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1509,20 +1647,22 @@
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G20" s="6">
-        <f>45/52</f>
-        <v>0.86538461538461542</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1533,20 +1673,26 @@
         <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G21" s="5">
-        <f>128/82</f>
+        <v>123</v>
+      </c>
+      <c r="G21" s="7">
+        <f>H21/I21</f>
         <v>1.5609756097560976</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="7">
+        <v>128</v>
+      </c>
+      <c r="I21" s="7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1557,20 +1703,26 @@
         <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G22" s="5">
-        <f>5979/147</f>
+        <v>125</v>
+      </c>
+      <c r="G22" s="7">
+        <f>H22/I22</f>
         <v>40.673469387755105</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="7">
+        <v>5979</v>
+      </c>
+      <c r="I22" s="7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1583,8 +1735,18 @@
       <c r="D23" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="7">
+        <f>H23/I23</f>
+        <v>24.35483870967742</v>
+      </c>
+      <c r="H23" s="7">
+        <v>2265</v>
+      </c>
+      <c r="I23" s="7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1595,23 +1757,29 @@
         <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G24" s="5">
-        <f>392/213</f>
+        <v>156</v>
+      </c>
+      <c r="G24" s="7">
+        <f>H24/I24</f>
         <v>1.84037558685446</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="7">
+        <v>392</v>
+      </c>
+      <c r="I24" s="7">
+        <v>213</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1622,23 +1790,31 @@
         <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G25" s="5">
-        <f>(752+1166)/(22+143)</f>
+        <v>158</v>
+      </c>
+      <c r="G25" s="7">
+        <f>H25/I25</f>
         <v>11.624242424242425</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="7">
+        <f>752+1166</f>
+        <v>1918</v>
+      </c>
+      <c r="I25" s="7">
+        <f>22+143</f>
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1649,19 +1825,19 @@
         <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1674,8 +1850,21 @@
       <c r="D27" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G27" s="7">
+        <f>H27/I27</f>
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="H27" s="7">
+        <v>240</v>
+      </c>
+      <c r="I27" s="7">
+        <v>66</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1686,22 +1875,19 @@
         <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1714,8 +1900,18 @@
       <c r="D29" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="7">
+        <f>H29/I29</f>
+        <v>72</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1440</v>
+      </c>
+      <c r="I29" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1726,20 +1922,26 @@
         <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G30" s="5">
-        <f>3203/119</f>
+        <v>188</v>
+      </c>
+      <c r="G30" s="7">
+        <f>H30/I30</f>
         <v>26.915966386554622</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="7">
+        <v>3203</v>
+      </c>
+      <c r="I30" s="7">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1750,23 +1952,29 @@
         <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G31" s="5">
-        <f>173/73</f>
+        <v>197</v>
+      </c>
+      <c r="G31" s="7">
+        <f>H31/I31</f>
         <v>2.3698630136986303</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H31" s="7">
+        <v>173</v>
+      </c>
+      <c r="I31" s="7">
+        <v>73</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1777,19 +1985,19 @@
         <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1800,23 +2008,29 @@
         <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G33" s="5">
-        <f>1190/745</f>
+        <v>165</v>
+      </c>
+      <c r="G33" s="7">
+        <f>H33/I33</f>
         <v>1.5973154362416107</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H33" s="7">
+        <v>1190</v>
+      </c>
+      <c r="I33" s="7">
+        <v>745</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1827,19 +2041,19 @@
         <v>63</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1850,23 +2064,29 @@
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G35" s="5">
-        <f>605/23</f>
+        <v>169</v>
+      </c>
+      <c r="G35" s="7">
+        <f>H35/I35</f>
         <v>26.304347826086957</v>
       </c>
-      <c r="H35" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="7">
+        <v>605</v>
+      </c>
+      <c r="I35" s="7">
+        <v>23</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1879,8 +2099,18 @@
       <c r="D36" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="7">
+        <f>H36/I36</f>
+        <v>25.5</v>
+      </c>
+      <c r="H36" s="7">
+        <v>2550</v>
+      </c>
+      <c r="I36" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1891,19 +2121,19 @@
         <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1916,8 +2146,21 @@
       <c r="D38" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="7">
+        <f>H38/I38</f>
+        <v>4.4052863436123344</v>
+      </c>
+      <c r="H38" s="7">
+        <v>1000</v>
+      </c>
+      <c r="I38" s="7">
+        <v>227</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1928,10 +2171,13 @@
         <v>75</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1942,20 +2188,26 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G40" s="5">
-        <f>206/12</f>
+        <v>135</v>
+      </c>
+      <c r="G40" s="7">
+        <f>H40/I40</f>
         <v>17.166666666666668</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="7">
+        <v>206</v>
+      </c>
+      <c r="I40" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1966,23 +2218,30 @@
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G41" s="5">
-        <f>(27222*9/60)/59</f>
+        <v>137</v>
+      </c>
+      <c r="G41" s="7">
+        <f>H41/I41</f>
         <v>69.208474576271186</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="7">
+        <f>(27222*9/60)</f>
+        <v>4083.3</v>
+      </c>
+      <c r="I41" s="7">
+        <v>59</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1993,20 +2252,26 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G42" s="5">
-        <f>129/11</f>
+        <v>139</v>
+      </c>
+      <c r="G42" s="7">
+        <f>H42/I42</f>
         <v>11.727272727272727</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="7">
+        <v>129</v>
+      </c>
+      <c r="I42" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2017,23 +2282,29 @@
         <v>85</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G43" s="5">
-        <f>203/132</f>
+        <v>182</v>
+      </c>
+      <c r="G43" s="7">
+        <f>H43/I43</f>
         <v>1.5378787878787878</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="7">
+        <v>203</v>
+      </c>
+      <c r="I43" s="7">
+        <v>132</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2044,19 +2315,19 @@
         <v>87</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2067,23 +2338,29 @@
         <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G45" s="5">
-        <f>81/16</f>
+        <v>192</v>
+      </c>
+      <c r="G45" s="7">
+        <f>H45/I45</f>
         <v>5.0625</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="7">
+        <v>81</v>
+      </c>
+      <c r="I45" s="7">
+        <v>16</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2094,20 +2371,27 @@
         <v>91</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G46" s="5">
-        <f>1361/63</f>
+        <v>180</v>
+      </c>
+      <c r="G46" s="7">
+        <f>H46/I46</f>
         <v>21.603174603174605</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H46" s="7">
+        <f>1361</f>
+        <v>1361</v>
+      </c>
+      <c r="I46" s="7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2118,19 +2402,19 @@
         <v>93</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2143,8 +2427,21 @@
       <c r="D48" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="7">
+        <f>H48/I48</f>
+        <v>15.055900621118013</v>
+      </c>
+      <c r="H48" s="7">
+        <v>2424</v>
+      </c>
+      <c r="I48" s="7">
+        <v>161</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2155,23 +2452,29 @@
         <v>97</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G49" s="5">
-        <f>128/72</f>
+        <v>188</v>
+      </c>
+      <c r="G49" s="7">
+        <f>H49/I49</f>
         <v>1.7777777777777777</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="7">
+        <v>128</v>
+      </c>
+      <c r="I49" s="7">
+        <v>72</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2184,8 +2487,21 @@
       <c r="D50" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G50" s="7">
+        <f>H50/I50</f>
+        <v>19.651162790697676</v>
+      </c>
+      <c r="H50" s="7">
+        <v>845</v>
+      </c>
+      <c r="I50" s="7">
+        <v>43</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2196,30 +2512,30 @@
         <v>101</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G51" s="5">
-        <f>238/21</f>
+        <v>176</v>
+      </c>
+      <c r="G51" s="7">
+        <f>H51/I51</f>
         <v>11.333333333333334</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>180</v>
+      <c r="H51" s="7">
+        <v>238</v>
+      </c>
+      <c r="I51" s="7">
+        <v>21</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Blocked"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G51" xr:uid="{1A7DA3E6-5977-4334-8866-21B6D35E68F1}"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{57FE75D0-032C-4AC1-83C8-CCA0DEF7DD1E}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{DAAD63D8-7315-40FF-A6E5-CCD3001C4F5B}"/>
@@ -2261,5 +2577,6 @@
     <hyperlink ref="C10" r:id="rId38" xr:uid="{8C6FF266-CAB6-4817-911C-DEA78521D44D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>